<commit_message>
Add navigation to main view after done
</commit_message>
<xml_diff>
--- a/Filtered_Rows.xlsx
+++ b/Filtered_Rows.xlsx
@@ -35,7 +35,7 @@
     <t>Termination Code</t>
   </si>
   <si>
-    <t>CB Dates</t>
+    <t>TC Dates</t>
   </si>
   <si>
     <t>Special Notes</t>
@@ -159,61 +159,61 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:b/>
       <main:sz val="11"/>
       <main:color indexed="8"/>
       <main:name val="Calibri"/>
     </font>
-    <font xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:b/>
       <main:sz val="11"/>
       <main:color indexed="8"/>
       <main:name val="Calibri"/>
     </font>
-    <font xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:b/>
       <main:sz val="11"/>
       <main:color indexed="8"/>
       <main:name val="Calibri"/>
     </font>
-    <font xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:b/>
       <main:sz val="11"/>
       <main:color indexed="8"/>
       <main:name val="Calibri"/>
     </font>
-    <font xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:b/>
       <main:sz val="11"/>
       <main:color indexed="8"/>
       <main:name val="Calibri"/>
     </font>
-    <font xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:b/>
       <main:sz val="11"/>
       <main:color indexed="8"/>
       <main:name val="Calibri"/>
     </font>
-    <font xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:b/>
       <main:sz val="11"/>
       <main:color indexed="8"/>
       <main:name val="Calibri"/>
     </font>
-    <font xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:b/>
       <main:sz val="11"/>
       <main:color indexed="8"/>
       <main:name val="Calibri"/>
     </font>
-    <font xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:b/>
       <main:sz val="11"/>
       <main:color indexed="8"/>
       <main:name val="Calibri"/>
     </font>
-    <font xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:b/>
       <main:sz val="11"/>
       <main:color indexed="8"/>
@@ -997,7 +997,7 @@
     <fill>
       <patternFill patternType="darkGray"/>
     </fill>
-    <fill xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+    <fill xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:patternFill patternType="solid">
         <main:fgColor indexed="13"/>
       </main:patternFill>
@@ -1017,16 +1017,16 @@
   </cellStyleXfs>
   <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true"/>
-    <xf xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true"/>
-    <xf xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true"/>
-    <xf xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true"/>
-    <xf xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true"/>
-    <xf xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true"/>
-    <xf xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true"/>
-    <xf xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true"/>
-    <xf xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true"/>
-    <xf xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>

</xml_diff>